<commit_message>
NPeres: v1.6. Changed connection to DB from pymysql to SQLAlchemy, added code to populate data in database. TODO: change timedelta values of failures DB columns before upload.
</commit_message>
<xml_diff>
--- a/cleaned_data_30_min.xlsx
+++ b/cleaned_data_30_min.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1021"/>
+  <dimension ref="A1:X1022"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80044,25 +80044,25 @@
         <v>44896.6875</v>
       </c>
       <c r="C1021" t="n">
-        <v>8.19278350515464</v>
+        <v>8.156020066889633</v>
       </c>
       <c r="D1021" t="n">
-        <v>71.73092783505155</v>
+        <v>71.14899665551839</v>
       </c>
       <c r="E1021" t="n">
-        <v>46.71855670103093</v>
+        <v>46.56153846153846</v>
       </c>
       <c r="F1021" t="n">
-        <v>-7.872164948453609</v>
+        <v>-7.745317725752508</v>
       </c>
       <c r="G1021" t="n">
-        <v>36.64948453608248</v>
+        <v>34.24247491638796</v>
       </c>
       <c r="H1021" t="n">
-        <v>2846.041237113402</v>
+        <v>2197.438127090301</v>
       </c>
       <c r="I1021" t="n">
-        <v>2.775257731958763</v>
+        <v>2.660367892976589</v>
       </c>
       <c r="J1021" t="n">
         <v>0</v>
@@ -80104,14 +80104,92 @@
       </c>
       <c r="V1021" t="inlineStr">
         <is>
-          <t>60_Hz</t>
+          <t>30_Hz</t>
         </is>
       </c>
       <c r="W1021" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X1021" t="n">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="1" t="n">
+        <v>4121</v>
+      </c>
+      <c r="B1022" s="2" t="n">
+        <v>44896.77083333334</v>
+      </c>
+      <c r="C1022" t="n">
+        <v>8.143155893536122</v>
+      </c>
+      <c r="D1022" t="n">
+        <v>69.32927756653991</v>
+      </c>
+      <c r="E1022" t="n">
+        <v>42.95361216730038</v>
+      </c>
+      <c r="F1022" t="n">
+        <v>-7.726045627376426</v>
+      </c>
+      <c r="G1022" t="n">
+        <v>28.07034220532319</v>
+      </c>
+      <c r="H1022" t="n">
+        <v>1273.077946768061</v>
+      </c>
+      <c r="I1022" t="n">
+        <v>2.317110266159696</v>
+      </c>
+      <c r="J1022" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1022" t="n">
+        <v>50</v>
+      </c>
+      <c r="L1022" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1022" t="n">
+        <v>80</v>
+      </c>
+      <c r="N1022" t="n">
+        <v>8625</v>
+      </c>
+      <c r="O1022" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="P1022" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q1022" t="b">
+        <v>0</v>
+      </c>
+      <c r="R1022" t="b">
+        <v>0</v>
+      </c>
+      <c r="S1022" t="b">
+        <v>0</v>
+      </c>
+      <c r="T1022" t="b">
+        <v>0</v>
+      </c>
+      <c r="U1022" t="inlineStr">
+        <is>
+          <t>2022-12-01</t>
+        </is>
+      </c>
+      <c r="V1022" t="inlineStr">
+        <is>
+          <t>30_Hz</t>
+        </is>
+      </c>
+      <c r="W1022" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="X1022" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>